<commit_message>
working model, debug needed
</commit_message>
<xml_diff>
--- a/RunControl.xlsx
+++ b/RunControl.xlsx
@@ -108,7 +108,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="107">
   <si>
     <t>runname</t>
   </si>
@@ -417,6 +417,18 @@
   </si>
   <si>
     <t>cola</t>
+  </si>
+  <si>
+    <t>policy</t>
+  </si>
+  <si>
+    <t>RS1_base</t>
+  </si>
+  <si>
+    <t>RS2_base</t>
+  </si>
+  <si>
+    <t>RS3_base</t>
   </si>
 </sst>
 </file>
@@ -1382,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AK7"/>
+  <dimension ref="A4:AJ10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1393,28 +1405,28 @@
     <col min="1" max="1" width="21.140625" customWidth="1"/>
     <col min="2" max="2" width="13.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="16" width="14.28515625" customWidth="1"/>
-    <col min="17" max="17" width="12.28515625" customWidth="1"/>
-    <col min="18" max="18" width="11.42578125" customWidth="1"/>
-    <col min="19" max="19" width="14.28515625" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.7109375" customWidth="1"/>
-    <col min="25" max="25" width="14" customWidth="1"/>
-    <col min="26" max="26" width="13.42578125" customWidth="1"/>
-    <col min="27" max="27" width="12.5703125" customWidth="1"/>
-    <col min="28" max="28" width="14.85546875" customWidth="1"/>
-    <col min="36" max="36" width="15.140625" customWidth="1"/>
-    <col min="37" max="37" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="14.28515625" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" customWidth="1"/>
+    <col min="24" max="24" width="14" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" customWidth="1"/>
+    <col min="26" max="26" width="12.5703125" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" customWidth="1"/>
+    <col min="35" max="35" width="15.140625" customWidth="1"/>
+    <col min="36" max="36" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:37" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1422,112 +1434,109 @@
         <v>95</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>89</v>
+        <v>15</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J4" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="J4" s="24" t="s">
         <v>99</v>
       </c>
+      <c r="K4" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="L4" s="1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="P4" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="P4" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="Q4" s="3" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="S4" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="S4" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="T4" s="4" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="U4" s="4" t="s">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="X4" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="X4" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="Y4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="Z4" s="6" t="s">
         <v>37</v>
       </c>
+      <c r="Z4" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="AA4" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="AB4" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="AC4" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AD4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE4" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="AE4" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="AF4" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AG4" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AH4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="AI4" s="9" t="s">
         <v>44</v>
       </c>
+      <c r="AI4" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="AJ4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="AK4" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -1537,26 +1546,26 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="E5" t="s">
         <v>100</v>
       </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
       <c r="G5" t="b">
         <v>1</v>
       </c>
       <c r="H5" t="b">
         <v>1</v>
       </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5">
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
         <v>0</v>
       </c>
       <c r="K5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="b">
         <v>1</v>
@@ -1564,74 +1573,71 @@
       <c r="M5" t="b">
         <v>1</v>
       </c>
-      <c r="N5" t="b">
-        <v>1</v>
+      <c r="N5">
+        <v>0.02</v>
       </c>
       <c r="O5">
-        <v>0.02</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
         <v>4</v>
       </c>
+      <c r="Q5" t="b">
+        <v>1</v>
+      </c>
       <c r="R5" t="b">
         <v>1</v>
       </c>
-      <c r="S5" t="b">
-        <v>1</v>
+      <c r="S5" t="s">
+        <v>101</v>
       </c>
       <c r="T5" t="s">
-        <v>101</v>
-      </c>
-      <c r="U5" t="s">
         <v>62</v>
       </c>
+      <c r="U5">
+        <v>12</v>
+      </c>
       <c r="V5">
-        <v>12</v>
+        <v>0.04</v>
       </c>
       <c r="W5">
-        <v>0.04</v>
+        <v>5</v>
       </c>
       <c r="X5">
-        <v>5</v>
-      </c>
-      <c r="Y5">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>35</v>
       </c>
       <c r="Z5" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="AA5" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB5" t="s">
         <v>21</v>
       </c>
+      <c r="AB5">
+        <v>7.2499999999999995E-2</v>
+      </c>
       <c r="AC5">
-        <v>7.2499999999999995E-2</v>
-      </c>
-      <c r="AD5">
         <v>7.9699999999999993E-2</v>
       </c>
-      <c r="AE5" s="7">
+      <c r="AD5" s="7">
         <v>0.12</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>45</v>
       </c>
       <c r="AF5" t="s">
         <v>45</v>
       </c>
-      <c r="AG5" t="s">
-        <v>45</v>
+      <c r="AG5">
+        <v>0.87622571862258425</v>
       </c>
       <c r="AH5">
-        <v>0.87622571862258425</v>
-      </c>
-      <c r="AI5">
         <v>0.92516191485799448</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1641,26 +1647,26 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="F6" t="s">
+      <c r="E6" t="s">
         <v>34</v>
       </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
       <c r="G6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="b">
         <v>1</v>
       </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6">
+      <c r="I6">
         <v>10</v>
       </c>
+      <c r="J6" t="b">
+        <v>0</v>
+      </c>
       <c r="K6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" t="b">
         <v>1</v>
@@ -1668,82 +1674,382 @@
       <c r="M6" t="b">
         <v>1</v>
       </c>
-      <c r="N6" t="b">
-        <v>1</v>
+      <c r="N6">
+        <v>0.02</v>
       </c>
       <c r="O6">
-        <v>0.02</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
         <v>4</v>
       </c>
+      <c r="Q6" t="b">
+        <v>1</v>
+      </c>
       <c r="R6" t="b">
         <v>1</v>
       </c>
-      <c r="S6" t="b">
-        <v>1</v>
+      <c r="S6" t="s">
+        <v>101</v>
       </c>
       <c r="T6" t="s">
-        <v>101</v>
-      </c>
-      <c r="U6" t="s">
         <v>62</v>
       </c>
+      <c r="U6">
+        <v>12</v>
+      </c>
       <c r="V6">
-        <v>12</v>
+        <v>0.04</v>
       </c>
       <c r="W6">
-        <v>0.04</v>
+        <v>5</v>
       </c>
       <c r="X6">
-        <v>5</v>
-      </c>
-      <c r="Y6">
-        <v>0</v>
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>35</v>
       </c>
       <c r="Z6" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="AA6" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB6" t="s">
         <v>21</v>
       </c>
+      <c r="AB6">
+        <v>7.2499999999999995E-2</v>
+      </c>
       <c r="AC6">
-        <v>7.2499999999999995E-2</v>
-      </c>
-      <c r="AD6">
         <v>7.9699999999999993E-2</v>
       </c>
-      <c r="AE6" s="7">
+      <c r="AD6" s="7">
         <v>0.12</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>45</v>
       </c>
       <c r="AF6" t="s">
         <v>45</v>
       </c>
-      <c r="AG6" t="s">
+      <c r="AG6">
+        <v>0.87622571862258425</v>
+      </c>
+      <c r="AH6">
+        <v>0.92516191485799448</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="AD7" s="7"/>
+    </row>
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>0</v>
+      </c>
+      <c r="K8" t="b">
+        <v>1</v>
+      </c>
+      <c r="L8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8" t="b">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0.02</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q8" t="b">
+        <v>1</v>
+      </c>
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>101</v>
+      </c>
+      <c r="T8" t="s">
+        <v>62</v>
+      </c>
+      <c r="U8">
+        <v>12</v>
+      </c>
+      <c r="V8">
+        <v>0.04</v>
+      </c>
+      <c r="W8">
+        <v>5</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB8">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="AC8">
+        <v>7.9699999999999993E-2</v>
+      </c>
+      <c r="AD8" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="AE8" t="s">
         <v>45</v>
       </c>
-      <c r="AH6">
+      <c r="AF8" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG8">
         <v>0.87622571862258425</v>
       </c>
-      <c r="AI6">
+      <c r="AH8">
         <v>0.92516191485799448</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="AE7" s="7"/>
+    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F9" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
+        <v>1</v>
+      </c>
+      <c r="H9" t="b">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>0</v>
+      </c>
+      <c r="K9" t="b">
+        <v>1</v>
+      </c>
+      <c r="L9" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9" t="b">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>0.02</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q9" t="b">
+        <v>1</v>
+      </c>
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
+        <v>101</v>
+      </c>
+      <c r="T9" t="s">
+        <v>62</v>
+      </c>
+      <c r="U9">
+        <v>12</v>
+      </c>
+      <c r="V9">
+        <v>0.04</v>
+      </c>
+      <c r="W9">
+        <v>5</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB9">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="AC9">
+        <v>7.9699999999999993E-2</v>
+      </c>
+      <c r="AD9" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG9">
+        <v>0.87622571862258425</v>
+      </c>
+      <c r="AH9">
+        <v>0.92516191485799448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" t="b">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="b">
+        <v>1</v>
+      </c>
+      <c r="L10" t="b">
+        <v>1</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0.02</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q10" t="b">
+        <v>1</v>
+      </c>
+      <c r="R10" t="b">
+        <v>1</v>
+      </c>
+      <c r="S10" t="s">
+        <v>101</v>
+      </c>
+      <c r="T10" t="s">
+        <v>62</v>
+      </c>
+      <c r="U10">
+        <v>12</v>
+      </c>
+      <c r="V10">
+        <v>0.04</v>
+      </c>
+      <c r="W10">
+        <v>5</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB10">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="AC10">
+        <v>7.9699999999999993E-2</v>
+      </c>
+      <c r="AD10" s="7">
+        <v>0.12</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG10">
+        <v>0.87622571862258425</v>
+      </c>
+      <c r="AH10">
+        <v>0.92516191485799448</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:I7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:H10">
       <formula1>"TRUE, FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA5:AA7">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z5:Z10">
       <formula1>"simple, internal"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1827,7 +2133,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>